<commit_message>
instalacion de bcrypt e implementacion para la creacion de usuarios en la contraseñas
</commit_message>
<xml_diff>
--- a/design/Generador de Archivos Json.xlsx
+++ b/design/Generador de Archivos Json.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alejandropascuale/Documentos/JavaScript/Proyecto Integrador/grupo_6_comamos/design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{042FC402-D732-704E-AEBE-6BCCD1F05650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51F54B6-75DF-FA45-A289-6FE06456DBB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{512CF241-1DAB-4F4D-ACDF-B2ED55074DC5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>idPlato</t>
   </si>
@@ -57,9 +57,6 @@
     <t>idRestaurante</t>
   </si>
   <si>
-    <t>P_00001</t>
-  </si>
-  <si>
     <t>CAPRESSE</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
   </si>
   <si>
     <t>Ensaladas</t>
-  </si>
-  <si>
-    <t>R_00001</t>
   </si>
   <si>
     <t>JSON</t>
@@ -426,8 +420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F84F4118-6433-F14C-94D5-B317B815A3D4}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,7 +433,8 @@
     <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="16" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="16" width="12.6640625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
@@ -493,35 +488,35 @@
         <v>"idRestaurante"</v>
       </c>
       <c r="R1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE("/img/products/",A2,".jpeg")</f>
-        <v>/img/products/P_00001.jpeg</v>
+        <v>/img/products/1.jpeg</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2">
         <v>300</v>
       </c>
-      <c r="G2" t="s">
-        <v>11</v>
+      <c r="G2">
+        <v>1</v>
       </c>
       <c r="I2" t="str">
         <f>""""&amp;A2&amp;""""</f>
-        <v>"P_00001"</v>
+        <v>"1"</v>
       </c>
       <c r="J2" t="str">
         <f t="shared" ref="J2:Q2" si="1">""""&amp;B2&amp;""""</f>
@@ -533,7 +528,7 @@
       </c>
       <c r="L2" t="str">
         <f t="shared" si="1"/>
-        <v>"/img/products/P_00001.jpeg"</v>
+        <v>"/img/products/1.jpeg"</v>
       </c>
       <c r="M2" t="str">
         <f t="shared" si="1"/>
@@ -545,11 +540,11 @@
       </c>
       <c r="O2" t="str">
         <f t="shared" si="1"/>
-        <v>"R_00001"</v>
+        <v>"1"</v>
       </c>
       <c r="R2" t="str">
         <f>CONCATENATE(I$1,":",I$2,",",J$1,":",J$2,",",K$1,":",K$2,",",L$1,":",L2,",",M$1,":",M2,",",N$1,":",N2,",",O$1,":",O2)</f>
-        <v>"idPlato":"P_00001","plato":"CAPRESSE","descripcion":"Mozzarella fior di late, tomate natural, albahaca fresca y olivas negras","imagen":"/img/products/P_00001.jpeg","categoria":"Ensaladas","precio":"300","idRestaurante":"R_00001"</v>
+        <v>"idPlato":"1","plato":"CAPRESSE","descripcion":"Mozzarella fior di late, tomate natural, albahaca fresca y olivas negras","imagen":"/img/products/1.jpeg","categoria":"Ensaladas","precio":"300","idRestaurante":"1"</v>
       </c>
     </row>
   </sheetData>

</xml_diff>